<commit_message>
Log in tests - update 2
</commit_message>
<xml_diff>
--- a/data/AutomationPracticeTestPlan.xlsx
+++ b/data/AutomationPracticeTestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Saška\Eclipse\Ajmo\Selenium project\SeleniumRepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B03983A-9408-46FC-BA91-C72968FCAAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AC7C4-1EBB-4B0E-9DDE-411292F3EEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
   <si>
     <t>Precondition:</t>
   </si>
@@ -538,9 +538,6 @@
     <t>Once the user submits entered email address, confirmation message for successfully sent request appears. When user checks if email arrived in outlook inbox, it doesn't appear in any folder - neither main or junk.</t>
   </si>
   <si>
-    <t>Bug 1.1 - Email with reset password link doesn't arrive in user's email after successfully submitting request</t>
-  </si>
-  <si>
     <t>Email with reset password link doesn't arrive in user's email after successfully submitting request</t>
   </si>
   <si>
@@ -571,6 +568,12 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Bug 1.1 - Inadequate message appears when user tries to log in with empty credentials</t>
+  </si>
+  <si>
+    <t>Bug 1.2 - Email with reset password link doesn't arrive in user's email after successfully submitting request</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -820,6 +823,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -839,11 +848,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1163,7 +1169,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,7 +1199,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -1206,7 +1212,7 @@
       <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="21" t="s">
         <v>49</v>
       </c>
@@ -1217,7 +1223,7 @@
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="21" t="s">
         <v>50</v>
       </c>
@@ -1225,10 +1231,12 @@
         <v>43</v>
       </c>
       <c r="D4" s="24"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="37" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="21" t="s">
         <v>51</v>
       </c>
@@ -1239,7 +1247,7 @@
       <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="21" t="s">
         <v>52</v>
       </c>
@@ -1250,7 +1258,7 @@
       <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="21" t="s">
         <v>53</v>
       </c>
@@ -1261,7 +1269,7 @@
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="21" t="s">
         <v>54</v>
       </c>
@@ -1272,7 +1280,7 @@
       <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="21" t="s">
         <v>55</v>
       </c>
@@ -1280,12 +1288,12 @@
         <v>45</v>
       </c>
       <c r="D9" s="24"/>
-      <c r="E9" s="36" t="s">
-        <v>94</v>
+      <c r="E9" s="29" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="21" t="s">
         <v>56</v>
       </c>
@@ -1296,7 +1304,7 @@
       <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="19" t="s">
         <v>47</v>
       </c>
@@ -1324,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1FFECC-C12E-4D4F-AFE2-9975F429C5EB}">
   <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,17 +1356,17 @@
       <c r="C1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="33"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="34"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1367,17 +1375,17 @@
       <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="32"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="31"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2143,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879D4113-4713-45C8-B4E3-9F4BAE6EA79F}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2163,19 +2171,19 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2233,7 +2241,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2241,33 +2249,33 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
+      <c r="A12" s="28"/>
       <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
-        <v>98</v>
+      <c r="A15" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2296,19 +2304,19 @@
         <v>88</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2377,7 +2385,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2385,13 +2393,13 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
+      <c r="A12" s="28"/>
       <c r="C12" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -2400,18 +2408,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
         <v>96</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="B15" t="s">
         <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My account tests - update 1 - My address, my personal information and my wishlist
</commit_message>
<xml_diff>
--- a/data/AutomationPracticeTestPlan.xlsx
+++ b/data/AutomationPracticeTestPlan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Saška\Eclipse\Ajmo\Selenium project\SeleniumRepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AC7C4-1EBB-4B0E-9DDE-411292F3EEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912695C7-1814-4DD6-92F3-B9BABD5B689F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Login Tests" sheetId="1" r:id="rId2"/>
     <sheet name="Bug 1.1" sheetId="4" r:id="rId3"/>
     <sheet name="Bug 1.2" sheetId="3" r:id="rId4"/>
+    <sheet name="My Account Tests" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="256">
   <si>
     <t>Precondition:</t>
   </si>
@@ -574,13 +575,1332 @@
   </si>
   <si>
     <t>Bug 1.2 - Email with reset password link doesn't arrive in user's email after successfully submitting request</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page after clicking on "My addresses" button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>formular page after clicking on "Add a new address" button</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user is able to save the new address after entering valid data in all mandatory fields</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to save the new address after entering invalid data in phone number field(s)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is unable to save the new address after entering invalid data in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Zip code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <t>TC3.01</t>
+  </si>
+  <si>
+    <t>TC3.02</t>
+  </si>
+  <si>
+    <t>TC3.03</t>
+  </si>
+  <si>
+    <t>TC3.04</t>
+  </si>
+  <si>
+    <t>TC3.05</t>
+  </si>
+  <si>
+    <t>Click on "My account" (User's first name and last name) main navigation tab</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page after clicking on "My addresses" button</t>
+    </r>
+  </si>
+  <si>
+    <t>TC2.01 - Verify that the user is successfully logged in after entering valid credentials - PASSED; User is successfully logged in.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "My addresses" button on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page and all user's addresses are shown.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>formular page after clicking on "Add a new address" button</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC2.01 - Verify that the user is successfully logged in after entering valid credentials - PASSED; User is successfully logged in.
+TC3.01 -  Verify that user is redirected to My addresses page after clicking on "My addresses" button - PASSED
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "Add a new address" button on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User is redirected to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page, new address formular shows</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter first name in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter last name in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter address in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter city name in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>City</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select state from </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dropdown menu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter zip code in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Zip/Postal Code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select country from </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dropdown menu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter phone number in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home phone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter phone number in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mobile phone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter address alias in your address section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Assign an address alias for future reference. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>input field</t>
+    </r>
+  </si>
+  <si>
+    <t>Aleksandra</t>
+  </si>
+  <si>
+    <t>Lakić</t>
+  </si>
+  <si>
+    <t>72  Peck Court</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>90017</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>949-429-8907</t>
+  </si>
+  <si>
+    <t>+949-429-8907</t>
+  </si>
+  <si>
+    <t>9494298907</t>
+  </si>
+  <si>
+    <t>Valid data 1:</t>
+  </si>
+  <si>
+    <t>Valid data 2:</t>
+  </si>
+  <si>
+    <t>Valid data 3:</t>
+  </si>
+  <si>
+    <t>$$phoneNumber</t>
+  </si>
+  <si>
+    <t>Invalid phone number:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is unable to save the new address after entering invalid data in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Zip code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Invalid zip code:</t>
+  </si>
+  <si>
+    <t>TC3.01 -  Verify that user is redirected to My addresses page after clicking on "My addresses" button - PASSED</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to save the new address with empty mandatory fields</t>
+  </si>
+  <si>
+    <t>TC3.06</t>
+  </si>
+  <si>
+    <t>Empty data:</t>
+  </si>
+  <si>
+    <t>Click on "Save" button</t>
+  </si>
+  <si>
+    <t>User is unable to save address without filling all mandatory fields. The following message appears:</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>New address 1</t>
+  </si>
+  <si>
+    <t>New address 2</t>
+  </si>
+  <si>
+    <t>New address 3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User has successfully saved new address.
+Created address appears on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <t>There is 1 error
+phone is invalid.</t>
+  </si>
+  <si>
+    <t>User is unable to save address without filling all mandatory fields with valid data. The following message appears:</t>
+  </si>
+  <si>
+    <t>There is 1 error
+The Zip/Postal code you've entered is invalid. It must follow this format: 00000</t>
+  </si>
+  <si>
+    <t>New address wrong</t>
+  </si>
+  <si>
+    <t>Addresses with aliases New address 1, New address 2, New address 3 or New address wrong do not exist in user's Addresses list</t>
+  </si>
+  <si>
+    <t>TC3.07</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to save the new address with already used alias</t>
+  </si>
+  <si>
+    <t>Used alias:</t>
+  </si>
+  <si>
+    <t>My address</t>
+  </si>
+  <si>
+    <t>There is 1 error
+The alias "My address" has already been used. Please select another one.</t>
+  </si>
+  <si>
+    <r>
+      <t>alias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>lastname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>firstname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>address1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>city</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> is required.</t>
+    </r>
+  </si>
+  <si>
+    <t>You must register at least one phone number.</t>
+  </si>
+  <si>
+    <t>This country requires you to chose a State.</t>
+  </si>
+  <si>
+    <t>The Zip/Postal code you've entered is invalid. It must follow this format: 00000</t>
+  </si>
+  <si>
+    <t>There are 8 errors
+alias is required.
+lastname is required.
+firstname is required.
+address1 is required.
+city is required.
+You must register at least one phone number.
+This country requires you to chose a State.
+The Zip/Postal code you've entered is invalid. It must follow this format: 00000</t>
+  </si>
+  <si>
+    <t>Verify that by clicking on "Update" button in address field, user is redirected to the address's formular page</t>
+  </si>
+  <si>
+    <t>Verify that by clicking on "Delete" button in address field, selected address is successfully deleted from addresses list</t>
+  </si>
+  <si>
+    <t>TC3.08</t>
+  </si>
+  <si>
+    <t>TC3.09</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TC3.01 -  Verify that user is redirected to My addresses page after clicking on "My addresses" button - PASSED; User is at the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>My addresses page</t>
+    </r>
+  </si>
+  <si>
+    <t>Click on "Update" button in the first address field</t>
+  </si>
+  <si>
+    <t>User is redirected to the first address's formular page and is able to edit any field and save address after entering all mandatory valid data.</t>
+  </si>
+  <si>
+    <t>Click on "Delete" button in the first address field</t>
+  </si>
+  <si>
+    <t>Click on "Yes" button in pop-up message</t>
+  </si>
+  <si>
+    <t>User has successfully deleted the chosen address;
+Deleted address doesn't appear in My addresses page</t>
+  </si>
+  <si>
+    <t>TC3.10</t>
+  </si>
+  <si>
+    <t>TC3.11</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter first name in personal information section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter last name in personal information section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter email address in personal information section's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter password in personal information section's
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current Password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter password in personal information section's
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <t>Valid data:</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>Jovana</t>
+  </si>
+  <si>
+    <t>Jovanović</t>
+  </si>
+  <si>
+    <t>Verify that personal information is successfully updated after valid data is entered in mandatory fields</t>
+  </si>
+  <si>
+    <t>Invalid current password:</t>
+  </si>
+  <si>
+    <t>TC3.12</t>
+  </si>
+  <si>
+    <t>TC3.13</t>
+  </si>
+  <si>
+    <t>Invalid new password:</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to update personal information after entering invalid new password</t>
+  </si>
+  <si>
+    <t>Invalid email address:</t>
+  </si>
+  <si>
+    <t>TC3.14</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to update personal information with empty data</t>
+  </si>
+  <si>
+    <t>User is unable to save personal information;
+The following message appears:</t>
+  </si>
+  <si>
+    <t>There is 1 error
+The password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t>There is 1 error
+The password and confirmation do not match.</t>
+  </si>
+  <si>
+    <t>There is 1 error
+This email address is not valid</t>
+  </si>
+  <si>
+    <t>aleksandralakic+1@livecom</t>
+  </si>
+  <si>
+    <t>Click on "My personal information" button</t>
+  </si>
+  <si>
+    <t>User is navigated to "My account" page</t>
+  </si>
+  <si>
+    <t>Verify that personal information is successfully updated only after correct current password is entered</t>
+  </si>
+  <si>
+    <t>User has successfully updated personal information;
+The following message appears:</t>
+  </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to update personal information after entering invalid email format</t>
+  </si>
+  <si>
+    <t>TC3.15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is redirecred to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">My wishlists </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page after clicking on "My wishlists" button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "My wishlists" button on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">My account </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User is redirecred to My wishlists page;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">My wishlists </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page elements are displayed</t>
+    </r>
+  </si>
+  <si>
+    <t>User is navigated to "My account" page;</t>
+  </si>
+  <si>
+    <t>TC3.14 - PASSED</t>
+  </si>
+  <si>
+    <t>TC3.16</t>
+  </si>
+  <si>
+    <t>TC3.17</t>
+  </si>
+  <si>
+    <t>TC3.18</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "Save" button in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New wishlist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> box</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fill </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">input field in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New wishlist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> box</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user is able to save new wishlist after wishlist name is entered</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to save new wishlist when wishlist name is not entered</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to save new wishlist if list with entered wishlist name already exists</t>
+  </si>
+  <si>
+    <t>My wishlist</t>
+  </si>
+  <si>
+    <t>New wishlist is not created, number of lists in table doesn't change</t>
+  </si>
+  <si>
+    <t>TC3.19</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add multiple wishlists using different names</t>
+  </si>
+  <si>
+    <t>Wishlist 1:</t>
+  </si>
+  <si>
+    <t>Wishlist 2:</t>
+  </si>
+  <si>
+    <t>Wishlist 3:</t>
+  </si>
+  <si>
+    <t>My wishlist 1</t>
+  </si>
+  <si>
+    <t>My wishlist 2</t>
+  </si>
+  <si>
+    <t>New wishlist is successfully created and shown in My wishlists table; Number of wishlists increases by 1;</t>
+  </si>
+  <si>
+    <t>New wishlist is successfully created and shown in My wishlists table; Number of wishlists increases by 3;</t>
+  </si>
+  <si>
+    <t>My wishlist 3</t>
+  </si>
+  <si>
+    <t>Verify that by clicking on the "x" icon, wishlist is successfully deleted</t>
+  </si>
+  <si>
+    <t>TC3.14, TC3.16 - PASSED</t>
+  </si>
+  <si>
+    <t>Click on "X" icon in row of wishlist chosen for removal</t>
+  </si>
+  <si>
+    <t>Click on "Yes" button on pop-up alert message</t>
+  </si>
+  <si>
+    <t>The chosen list is successfully removed;
+Number of lists presented in the table decreased by 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,6 +1958,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -665,7 +1996,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -691,15 +2022,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -765,12 +2087,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -806,20 +2218,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -829,13 +2240,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,8 +2282,58 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1166,13 +2650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3459B804-6861-4AD7-85C4-B4C580902825}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -1181,147 +2665,338 @@
     <col min="5" max="5" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1">
+      <c r="A1" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="61" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:5" ht="28.8">
+      <c r="A2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="21" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="42"/>
+      <c r="B3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.8">
+      <c r="A4" s="42"/>
+      <c r="B4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="37" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="21" t="s">
+    <row r="5" spans="1:5" ht="28.8">
+      <c r="A5" s="42"/>
+      <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="21" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="42"/>
+      <c r="B6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="21" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8">
+      <c r="A7" s="42"/>
+      <c r="B7" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="21" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8">
+      <c r="A8" s="42"/>
+      <c r="B8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="21" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" ht="43.2">
+      <c r="A9" s="42"/>
+      <c r="B9" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="29" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="28" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="1:5" ht="43.2">
+      <c r="A10" s="42"/>
+      <c r="B10" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="19" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A11" s="58"/>
+      <c r="B11" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8">
+      <c r="A12" s="65" t="s">
         <v>58</v>
       </c>
+      <c r="B12" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8">
+      <c r="A13" s="66"/>
+      <c r="B13" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="41"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.8">
+      <c r="A14" s="66"/>
+      <c r="B14" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:5" ht="28.8">
+      <c r="A15" s="66"/>
+      <c r="B15" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:5" ht="28.8">
+      <c r="A16" s="66"/>
+      <c r="B16" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:5" ht="28.8">
+      <c r="A17" s="66"/>
+      <c r="B17" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.8">
+      <c r="A18" s="66"/>
+      <c r="B18" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.8">
+      <c r="A19" s="66"/>
+      <c r="B19" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" ht="28.8">
+      <c r="A20" s="66"/>
+      <c r="B20" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="28.8">
+      <c r="A21" s="66"/>
+      <c r="B21" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" ht="28.8">
+      <c r="A22" s="66"/>
+      <c r="B22" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8">
+      <c r="A23" s="66"/>
+      <c r="B23" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.8">
+      <c r="A24" s="66"/>
+      <c r="B24" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8">
+      <c r="A25" s="66"/>
+      <c r="B25" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8">
+      <c r="A26" s="66"/>
+      <c r="B26" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8">
+      <c r="A27" s="66"/>
+      <c r="B27" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" ht="28.8">
+      <c r="A28" s="66"/>
+      <c r="B28" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8">
+      <c r="A29" s="66"/>
+      <c r="B29" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A30" s="67"/>
+      <c r="B30" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1332,11 +3007,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1FFECC-C12E-4D4F-AFE2-9975F429C5EB}">
   <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.21875" bestFit="1" customWidth="1"/>
@@ -1348,7 +3023,7 @@
     <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1356,38 +3031,38 @@
       <c r="C1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="36"/>
-    </row>
-    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H1" s="46"/>
+    </row>
+    <row r="2" spans="1:29" ht="43.2">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="H2" s="43"/>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1398,15 +3073,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29">
       <c r="B4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1429,7 +3104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1443,7 +3118,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1467,7 +3142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1491,7 +3166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1499,7 +3174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="100.8">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +3197,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="43.2">
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1539,7 +3214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -1564,7 +3239,7 @@
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +3274,7 @@
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
     </row>
-    <row r="16" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="72">
       <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
@@ -1607,7 +3282,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1618,15 +3293,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18">
       <c r="B18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -1634,7 +3309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1643,7 +3318,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1654,7 +3329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1665,7 +3340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1673,7 +3348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="86.4">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
@@ -1681,7 +3356,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1701,7 +3376,7 @@
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -1709,7 +3384,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="43.2">
       <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
@@ -1717,7 +3392,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18">
       <c r="A31" s="4" t="s">
         <v>0</v>
       </c>
@@ -1728,12 +3403,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18">
       <c r="B32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +3416,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1750,7 +3425,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1761,7 +3436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1772,7 +3447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="43.2">
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
@@ -1780,7 +3455,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24">
       <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
@@ -1788,7 +3463,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -1814,7 +3489,7 @@
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24">
       <c r="A43" s="4" t="s">
         <v>26</v>
       </c>
@@ -1822,7 +3497,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="57.6">
       <c r="A44" s="4" t="s">
         <v>62</v>
       </c>
@@ -1830,7 +3505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24">
       <c r="A46" s="4" t="s">
         <v>0</v>
       </c>
@@ -1841,7 +3516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -1849,7 +3524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1858,7 +3533,7 @@
       </c>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1867,10 +3542,10 @@
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24">
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" ht="28.8">
       <c r="A52" s="4" t="s">
         <v>8</v>
       </c>
@@ -1878,7 +3553,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -1904,7 +3579,7 @@
       <c r="W53" s="15"/>
       <c r="X53" s="15"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24">
       <c r="A54" s="4" t="s">
         <v>26</v>
       </c>
@@ -1915,7 +3590,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" ht="86.4">
       <c r="A55" s="4" t="s">
         <v>62</v>
       </c>
@@ -1926,7 +3601,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24">
       <c r="A57" s="4" t="s">
         <v>0</v>
       </c>
@@ -1937,12 +3612,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24">
       <c r="B58" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24">
       <c r="A59" s="4" t="s">
         <v>3</v>
       </c>
@@ -1953,7 +3628,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1962,7 +3637,7 @@
       </c>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1971,7 +3646,7 @@
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24">
       <c r="A62">
         <v>3</v>
       </c>
@@ -1985,7 +3660,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24">
       <c r="A63">
         <v>4</v>
       </c>
@@ -1993,7 +3668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" ht="86.4">
       <c r="A64" s="4" t="s">
         <v>8</v>
       </c>
@@ -2004,7 +3679,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" ht="43.2">
       <c r="A65" s="4"/>
       <c r="C65" s="3" t="s">
         <v>80</v>
@@ -2013,7 +3688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -2039,7 +3714,7 @@
       <c r="W66" s="12"/>
       <c r="X66" s="12"/>
     </row>
-    <row r="67" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" ht="28.8">
       <c r="A67" s="4" t="s">
         <v>62</v>
       </c>
@@ -2048,11 +3723,11 @@
       </c>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24">
       <c r="A69" s="4" t="s">
         <v>0</v>
       </c>
@@ -2063,23 +3738,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24">
       <c r="B70" t="s">
         <v>59</v>
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24">
       <c r="B71" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24">
       <c r="A73" s="4" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +3763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24">
       <c r="A74">
         <v>1</v>
       </c>
@@ -2099,7 +3774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24">
       <c r="B75" s="6" t="s">
         <v>38</v>
       </c>
@@ -2107,7 +3782,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24">
       <c r="A76">
         <v>2</v>
       </c>
@@ -2116,7 +3791,7 @@
       </c>
       <c r="C76" s="2"/>
     </row>
-    <row r="78" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" ht="43.2">
       <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
@@ -2155,39 +3830,39 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:3" ht="43.2">
+      <c r="A2" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:3" ht="43.2">
+      <c r="A3" s="27" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -2197,15 +3872,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="26" t="s">
         <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2214,7 +3889,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2223,7 +3898,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2232,7 +3907,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2240,38 +3915,38 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:3" ht="43.2">
+      <c r="A11" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+    <row r="12" spans="1:3" ht="43.2">
+      <c r="A12" s="27"/>
       <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:3" ht="72">
+      <c r="A13" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B15" t="s">
@@ -2292,39 +3967,39 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:3" ht="43.2">
+      <c r="A2" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:3" ht="43.2">
+      <c r="A3" s="27" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -2334,20 +4009,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="26" t="s">
         <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2356,7 +4031,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2365,7 +4040,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2376,7 +4051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2384,38 +4059,38 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:3" ht="72">
+      <c r="A11" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+    <row r="12" spans="1:3" ht="43.2">
+      <c r="A12" s="27"/>
       <c r="C12" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:3" ht="72">
+      <c r="A13" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B15" t="s">
@@ -2429,4 +4104,1547 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5914067F-A3D6-4F1D-8A65-E4F056E7FEB8}">
+  <dimension ref="A1:R139"/>
+  <sheetViews>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:17" ht="57.6">
+      <c r="A2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="43.2" customHeight="1">
+      <c r="B4" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="48"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="30"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="28.8">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="43.2">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="57.6">
+      <c r="A13" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="58.2" customHeight="1">
+      <c r="B15" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="48"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.4" customHeight="1">
+      <c r="A16" s="30"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="28.8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="28.8">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="43.2">
+      <c r="A22" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="46"/>
+      <c r="I24" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="58.2" customHeight="1">
+      <c r="A25" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" s="44"/>
+      <c r="I25" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="30"/>
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="28.8">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" ht="28.8">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" ht="28.8">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="28.8">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" ht="28.8">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" ht="28.8">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" ht="28.8">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" ht="43.2">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="72">
+      <c r="A44" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="172.8">
+      <c r="F45" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J47" s="49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="57.6">
+      <c r="A48" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="J48" s="49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" s="49" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+      <c r="J50" s="49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="39"/>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="J51" s="50" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J52" s="50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="20.399999999999999">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>188</v>
+      </c>
+      <c r="J53" s="50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="43.2">
+      <c r="A55" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="72">
+      <c r="A58" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="39"/>
+      <c r="B61" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="43.2">
+      <c r="A66" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="G68" s="39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="57.6">
+      <c r="A69" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="F69" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="G69" s="38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="B72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="39"/>
+      <c r="B73" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:9" ht="28.8">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:9" ht="28.8">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" ht="28.8">
+      <c r="A79">
+        <v>4</v>
+      </c>
+      <c r="B79" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:9" ht="28.8">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" ht="28.8">
+      <c r="A81">
+        <v>6</v>
+      </c>
+      <c r="B81" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" ht="57.6">
+      <c r="A84" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="C84" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="D84" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="E84" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="F84" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="G84" s="40" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="43.2">
+      <c r="B85" s="2"/>
+      <c r="C85" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="F85" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" s="39" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="43.2">
+      <c r="A88" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="39"/>
+      <c r="B92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="28.8">
+      <c r="A97" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="E99" s="39" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="57.6">
+      <c r="A100" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="B103" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="39"/>
+      <c r="B104" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="B105" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="1:8" ht="57.6">
+      <c r="A111" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D111" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="E111" s="40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="12"/>
+      <c r="B112" s="63"/>
+      <c r="C112" s="63"/>
+      <c r="D112" s="63"/>
+      <c r="E112" s="63"/>
+      <c r="F112" s="12"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="2"/>
+      <c r="C113" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="D113" s="46"/>
+      <c r="E113" s="46"/>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C114" s="64" t="s">
+        <v>242</v>
+      </c>
+      <c r="D114" s="64"/>
+      <c r="E114" s="64"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="B117" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C117" s="2"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="39"/>
+      <c r="B118" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="B119" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="D120" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="E120" s="39" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C121" s="2"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122">
+        <v>2</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="1:8" ht="27" customHeight="1">
+      <c r="A125" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="D125" s="47"/>
+      <c r="E125" s="47"/>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="12"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C127" s="39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="43.2">
+      <c r="A128" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C128" s="38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="B131" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="39"/>
+      <c r="B132" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C132" s="2"/>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="B133" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C133" s="2"/>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="28.8">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="57.6">
+      <c r="A139" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C24:E24"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C79" r:id="rId1" xr:uid="{A14C5E75-288F-4637-9146-BEA59811E139}"/>
+    <hyperlink ref="D79" r:id="rId2" xr:uid="{283E04EA-50E3-4445-B9B4-EB8F77FB15DA}"/>
+    <hyperlink ref="E79" r:id="rId3" xr:uid="{92A45497-1FC0-4F5D-97B3-AFB46BBA88B1}"/>
+    <hyperlink ref="F79" r:id="rId4" xr:uid="{EEEDC609-6145-4D66-A131-A26B5BA64498}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My account section - update 2
</commit_message>
<xml_diff>
--- a/data/AutomationPracticeTestPlan.xlsx
+++ b/data/AutomationPracticeTestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Saška\Eclipse\Ajmo\Selenium project\SeleniumRepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912695C7-1814-4DD6-92F3-B9BABD5B689F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260F424-548D-4A88-A25D-5F5E951B9E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="257">
   <si>
     <t>Precondition:</t>
   </si>
@@ -1894,6 +1894,9 @@
   <si>
     <t>The chosen list is successfully removed;
 Number of lists presented in the table decreased by 1</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1973,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1992,6 +1995,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2182,7 +2191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2269,25 +2278,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2311,9 +2301,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2323,8 +2310,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2334,6 +2325,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2652,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3459B804-6861-4AD7-85C4-B4C580902825}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2666,24 +2676,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="53" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="57" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -2696,7 +2706,7 @@
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="42"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="20" t="s">
         <v>49</v>
       </c>
@@ -2707,7 +2717,7 @@
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="28.8">
-      <c r="A4" s="42"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="20" t="s">
         <v>50</v>
       </c>
@@ -2720,7 +2730,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8">
-      <c r="A5" s="42"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
@@ -2731,7 +2741,7 @@
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" ht="28.8">
-      <c r="A6" s="42"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="20" t="s">
         <v>52</v>
       </c>
@@ -2742,7 +2752,7 @@
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" ht="28.8">
-      <c r="A7" s="42"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="20" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2763,7 @@
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" ht="28.8">
-      <c r="A8" s="42"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="20" t="s">
         <v>54</v>
       </c>
@@ -2764,7 +2774,7 @@
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="43.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="20" t="s">
         <v>55</v>
       </c>
@@ -2777,7 +2787,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="20" t="s">
         <v>56</v>
       </c>
@@ -2789,17 +2799,17 @@
     </row>
     <row r="11" spans="1:5" ht="29.4" thickBot="1">
       <c r="A11" s="58"/>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
     </row>
     <row r="12" spans="1:5" ht="28.8">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="59" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -2811,7 +2821,7 @@
       <c r="D12" s="41"/>
     </row>
     <row r="13" spans="1:5" ht="28.8">
-      <c r="A13" s="66"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="34" t="s">
         <v>112</v>
       </c>
@@ -2821,7 +2831,7 @@
       <c r="D13" s="41"/>
     </row>
     <row r="14" spans="1:5" ht="28.8">
-      <c r="A14" s="66"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="34" t="s">
         <v>113</v>
       </c>
@@ -2831,7 +2841,7 @@
       <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:5" ht="28.8">
-      <c r="A15" s="66"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="34" t="s">
         <v>114</v>
       </c>
@@ -2841,7 +2851,7 @@
       <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:5" ht="28.8">
-      <c r="A16" s="66"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="34" t="s">
         <v>115</v>
       </c>
@@ -2851,7 +2861,7 @@
       <c r="D16" s="41"/>
     </row>
     <row r="17" spans="1:5" ht="28.8">
-      <c r="A17" s="66"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="34" t="s">
         <v>155</v>
       </c>
@@ -2861,7 +2871,7 @@
       <c r="D17" s="41"/>
     </row>
     <row r="18" spans="1:5" ht="28.8">
-      <c r="A18" s="66"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="34" t="s">
         <v>169</v>
       </c>
@@ -2871,7 +2881,7 @@
       <c r="D18" s="41"/>
     </row>
     <row r="19" spans="1:5" ht="28.8">
-      <c r="A19" s="66"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="34" t="s">
         <v>185</v>
       </c>
@@ -2881,18 +2891,18 @@
       <c r="D19" s="41"/>
     </row>
     <row r="20" spans="1:5" ht="28.8">
-      <c r="A20" s="66"/>
-      <c r="B20" s="56" t="s">
+      <c r="A20" s="60"/>
+      <c r="B20" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="50" t="s">
         <v>184</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="28.8">
-      <c r="A21" s="66"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="34" t="s">
         <v>193</v>
       </c>
@@ -2902,7 +2912,7 @@
       <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:5" ht="28.8">
-      <c r="A22" s="66"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="34" t="s">
         <v>194</v>
       </c>
@@ -2912,7 +2922,7 @@
       <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:5" ht="28.8">
-      <c r="A23" s="66"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="34" t="s">
         <v>207</v>
       </c>
@@ -2922,7 +2932,7 @@
       <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:5" ht="28.8">
-      <c r="A24" s="66"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="34" t="s">
         <v>208</v>
       </c>
@@ -2932,19 +2942,19 @@
       <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:5" ht="28.8">
-      <c r="A25" s="66"/>
-      <c r="B25" s="56" t="s">
+      <c r="A25" s="60"/>
+      <c r="B25" s="49" t="s">
         <v>212</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="50" t="s">
         <v>213</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="28.8">
-      <c r="A26" s="66"/>
-      <c r="B26" s="56" t="s">
+      <c r="A26" s="60"/>
+      <c r="B26" s="49" t="s">
         <v>212</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2953,8 +2963,8 @@
       <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:5" ht="28.8">
-      <c r="A27" s="66"/>
-      <c r="B27" s="56" t="s">
+      <c r="A27" s="60"/>
+      <c r="B27" s="49" t="s">
         <v>212</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2963,8 +2973,8 @@
       <c r="D27" s="41"/>
     </row>
     <row r="28" spans="1:5" ht="28.8">
-      <c r="A28" s="66"/>
-      <c r="B28" s="56" t="s">
+      <c r="A28" s="60"/>
+      <c r="B28" s="49" t="s">
         <v>212</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2973,8 +2983,8 @@
       <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:5" ht="28.8">
-      <c r="A29" s="66"/>
-      <c r="B29" s="56" t="s">
+      <c r="A29" s="60"/>
+      <c r="B29" s="49" t="s">
         <v>212</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2983,15 +2993,15 @@
       <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A30" s="67"/>
-      <c r="B30" s="52" t="s">
+      <c r="A30" s="61"/>
+      <c r="B30" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="53" t="s">
+      <c r="C30" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="55"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3031,17 +3041,17 @@
       <c r="C1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="45"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="46"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:29" ht="43.2">
       <c r="A2" s="4" t="s">
@@ -3050,17 +3060,17 @@
       <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="43"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="4" t="s">
@@ -4108,10 +4118,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5914067F-A3D6-4F1D-8A65-E4F056E7FEB8}">
-  <dimension ref="A1:R139"/>
+  <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4157,10 +4167,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="43.2" customHeight="1">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="30"/>
@@ -4241,10 +4251,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="58.2" customHeight="1">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="66"/>
     </row>
     <row r="16" spans="1:17" ht="14.4" customHeight="1">
       <c r="A16" s="30"/>
@@ -4310,18 +4320,18 @@
       <c r="A24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="46"/>
+      <c r="H24" s="65"/>
       <c r="I24" s="33" t="s">
         <v>155</v>
       </c>
@@ -4333,18 +4343,18 @@
       <c r="A25" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
       <c r="F25" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="44"/>
+      <c r="H25" s="63"/>
       <c r="I25" s="32" t="s">
         <v>170</v>
       </c>
@@ -4556,7 +4566,9 @@
       <c r="I36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J36" s="2"/>
+      <c r="J36" s="2" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="28.8">
       <c r="A37">
@@ -4616,7 +4628,9 @@
       <c r="I38" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="J38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="28.8">
       <c r="A39">
@@ -4706,11 +4720,11 @@
       <c r="A44" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="68" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
       <c r="F44" s="3" t="s">
         <v>165</v>
       </c>
@@ -4754,7 +4768,7 @@
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
-      <c r="J46" s="51" t="s">
+      <c r="J46" s="44" t="s">
         <v>174</v>
       </c>
       <c r="K46" s="12"/>
@@ -4766,7 +4780,7 @@
       <c r="C47" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="J47" s="49" t="s">
+      <c r="J47" s="42" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4777,7 +4791,7 @@
       <c r="C48" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="J48" s="49" t="s">
+      <c r="J48" s="42" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4791,7 +4805,7 @@
       <c r="C49" t="s">
         <v>2</v>
       </c>
-      <c r="J49" s="49" t="s">
+      <c r="J49" s="42" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4799,7 +4813,7 @@
       <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="J50" s="49" t="s">
+      <c r="J50" s="42" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4808,7 +4822,7 @@
       <c r="B51" t="s">
         <v>187</v>
       </c>
-      <c r="J51" s="50" t="s">
+      <c r="J51" s="43" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4816,7 +4830,7 @@
       <c r="A52" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="J52" s="50" t="s">
+      <c r="J52" s="43" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4827,7 +4841,7 @@
       <c r="B53" t="s">
         <v>188</v>
       </c>
-      <c r="J53" s="50" t="s">
+      <c r="J53" s="43" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4920,14 +4934,14 @@
       </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
+      <c r="A67" s="56"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
+      <c r="H67" s="56"/>
       <c r="I67" s="12"/>
     </row>
     <row r="68" spans="1:9">
@@ -5186,14 +5200,14 @@
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
+      <c r="A86" s="56"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="56"/>
+      <c r="D86" s="56"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="56"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="56"/>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="39" t="s">
@@ -5405,10 +5419,10 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="12"/>
-      <c r="B112" s="63"/>
-      <c r="C112" s="63"/>
-      <c r="D112" s="63"/>
-      <c r="E112" s="63"/>
+      <c r="B112" s="55"/>
+      <c r="C112" s="55"/>
+      <c r="D112" s="55"/>
+      <c r="E112" s="55"/>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
@@ -5418,21 +5432,21 @@
         <v>26</v>
       </c>
       <c r="B113" s="2"/>
-      <c r="C113" s="46" t="s">
+      <c r="C113" s="65" t="s">
         <v>241</v>
       </c>
-      <c r="D113" s="46"/>
-      <c r="E113" s="46"/>
+      <c r="D113" s="65"/>
+      <c r="E113" s="65"/>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C114" s="64" t="s">
+      <c r="C114" s="67" t="s">
         <v>242</v>
       </c>
-      <c r="D114" s="64"/>
-      <c r="E114" s="64"/>
+      <c r="D114" s="67"/>
+      <c r="E114" s="67"/>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" s="39" t="s">
@@ -5526,11 +5540,11 @@
         <v>8</v>
       </c>
       <c r="B125" s="2"/>
-      <c r="C125" s="47" t="s">
+      <c r="C125" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="D125" s="47"/>
-      <c r="E125" s="47"/>
+      <c r="D125" s="68"/>
+      <c r="E125" s="68"/>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" s="12"/>
@@ -5558,7 +5572,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:8">
       <c r="A130" s="39" t="s">
         <v>0</v>
       </c>
@@ -5569,31 +5583,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:8">
       <c r="B131" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:8">
       <c r="A132" s="39"/>
       <c r="B132" s="2" t="s">
         <v>252</v>
       </c>
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:8">
       <c r="B133" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:8">
       <c r="A134" s="39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:8">
       <c r="A135">
         <v>1</v>
       </c>
@@ -5601,7 +5615,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="28.8">
+    <row r="136" spans="1:8" ht="28.8">
       <c r="A136">
         <v>2</v>
       </c>
@@ -5609,7 +5623,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:8">
       <c r="A137">
         <v>3</v>
       </c>
@@ -5617,7 +5631,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="57.6">
+    <row r="139" spans="1:8" ht="57.6">
       <c r="A139" s="39" t="s">
         <v>8</v>
       </c>
@@ -5625,9 +5639,18 @@
         <v>255</v>
       </c>
     </row>
+    <row r="140" spans="1:8">
+      <c r="A140" s="56"/>
+      <c r="B140" s="56"/>
+      <c r="C140" s="56"/>
+      <c r="D140" s="56"/>
+      <c r="E140" s="56"/>
+      <c r="F140" s="56"/>
+      <c r="G140" s="56"/>
+      <c r="H140" s="56"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C113:E113"/>
     <mergeCell ref="C114:E114"/>
     <mergeCell ref="C125:E125"/>
     <mergeCell ref="G25:H25"/>
@@ -5637,6 +5660,7 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C113:E113"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C79" r:id="rId1" xr:uid="{A14C5E75-288F-4637-9146-BEA59811E139}"/>

</xml_diff>

<commit_message>
Add to cart tests - update 1
</commit_message>
<xml_diff>
--- a/data/AutomationPracticeTestPlan.xlsx
+++ b/data/AutomationPracticeTestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Saška\Eclipse\Ajmo\Selenium project\SeleniumRepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260F424-548D-4A88-A25D-5F5E951B9E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E35589-3D03-49FD-99F4-8500098D3174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{5B8095E8-B6E4-44A1-8259-E88295B322A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Bug 1.1" sheetId="4" r:id="rId3"/>
     <sheet name="Bug 1.2" sheetId="3" r:id="rId4"/>
     <sheet name="My Account Tests" sheetId="5" r:id="rId5"/>
+    <sheet name="Add To Cart Tests" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="299">
   <si>
     <t>Precondition:</t>
   </si>
@@ -1897,6 +1898,273 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>MY ADDRESSES TESTS</t>
+  </si>
+  <si>
+    <t>PERSONAL INFORMATION TESTS</t>
+  </si>
+  <si>
+    <t>MY WISHLISTS TESTS</t>
+  </si>
+  <si>
+    <t>Add to cart</t>
+  </si>
+  <si>
+    <t>TC4.01</t>
+  </si>
+  <si>
+    <t>TC4.02</t>
+  </si>
+  <si>
+    <t>TC4.03</t>
+  </si>
+  <si>
+    <t>TC4.04</t>
+  </si>
+  <si>
+    <t>Verify that the product is added to cart after clicking on "Add to cart" button</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add multiple different products to cart by clicking on "Add to cart" button on different products</t>
+  </si>
+  <si>
+    <t>TC4.05</t>
+  </si>
+  <si>
+    <t>TC4.06</t>
+  </si>
+  <si>
+    <t>Verify that user is able to remove product from the cart by clicking on trash can icon button</t>
+  </si>
+  <si>
+    <t>Click on "Cart" button from home page</t>
+  </si>
+  <si>
+    <t>TC4.01 - adding product to cart - PASSED</t>
+  </si>
+  <si>
+    <t>Click on "Proceed to checkout" button from pop-up window</t>
+  </si>
+  <si>
+    <t>Verify that user is able to increase quantity of chosen product once it's added to cart by clicking on "+" button</t>
+  </si>
+  <si>
+    <t>Verify that user is able to decrease quantity of chosen product once it's added to cart by clicking on "-" button</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "+" button next to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The quantity of added product has increased by 1. New, higher product amount is displayed in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The quantity of added product has decreased by 1. New, lower product amount is displayed in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on "-" button next to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input field</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user is able to change quantity of chosen product to valid amount once it's added to cart by keyboard input</t>
+  </si>
+  <si>
+    <t>TC4.07</t>
+  </si>
+  <si>
+    <t>TC4.08</t>
+  </si>
+  <si>
+    <t>TC4.01 - adding product to cart - PASSED;
+TC4.04 precondition: quantity added product equals 1</t>
+  </si>
+  <si>
+    <t>Verify that when quantity is decreased to 0 by clicking on "-" button, cart empties</t>
+  </si>
+  <si>
+    <t>The quantity of added product has decreased by 1. Cart is empty and the following message appears:</t>
+  </si>
+  <si>
+    <t>Your shopping cart is empty.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter any integer in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Quantity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>input field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The quantity of added product has been set to inputed number. New, product amount is displayed in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <t>Positive integer:</t>
+  </si>
+  <si>
+    <t>Negative integer:</t>
+  </si>
+  <si>
+    <t>Zero:</t>
+  </si>
+  <si>
+    <t>Cart is empty and the following message appears:</t>
+  </si>
+  <si>
+    <t>User is unable to successfuly set quantity to negative number. The quantity of added product stays the same like before input.</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to successfully change quantity of chosen product to negative number once it's added to cart by keyboard input</t>
+  </si>
+  <si>
+    <t>Click on "Add to cart" button of product with following index (check Test data column)</t>
+  </si>
+  <si>
+    <t>Test data :</t>
+  </si>
+  <si>
+    <t>ADD TO CART TESTS</t>
+  </si>
+  <si>
+    <t>The selected product is added and shown in cart page; Product quantity box in cart page contains following text:</t>
+  </si>
+  <si>
+    <t>Your shopping cart contains: 1 Product</t>
   </si>
 </sst>
 </file>
@@ -2191,7 +2459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2263,7 +2531,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2311,6 +2578,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2336,15 +2610,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2660,10 +2938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3459B804-6861-4AD7-85C4-B4C580902825}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2676,24 +2954,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -2706,7 +2984,7 @@
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="57"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="20" t="s">
         <v>49</v>
       </c>
@@ -2717,7 +2995,7 @@
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="28.8">
-      <c r="A4" s="57"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="20" t="s">
         <v>50</v>
       </c>
@@ -2730,7 +3008,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8">
-      <c r="A5" s="57"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
@@ -2741,7 +3019,7 @@
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" ht="28.8">
-      <c r="A6" s="57"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="20" t="s">
         <v>52</v>
       </c>
@@ -2752,7 +3030,7 @@
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" ht="28.8">
-      <c r="A7" s="57"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="20" t="s">
         <v>53</v>
       </c>
@@ -2763,7 +3041,7 @@
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" ht="28.8">
-      <c r="A8" s="57"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="20" t="s">
         <v>54</v>
       </c>
@@ -2774,7 +3052,7 @@
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="43.2">
-      <c r="A9" s="57"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="20" t="s">
         <v>55</v>
       </c>
@@ -2787,7 +3065,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2">
-      <c r="A10" s="57"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="20" t="s">
         <v>56</v>
       </c>
@@ -2798,18 +3076,18 @@
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A11" s="58"/>
-      <c r="B11" s="51" t="s">
+      <c r="A11" s="60"/>
+      <c r="B11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
     </row>
     <row r="12" spans="1:5" ht="28.8">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="61" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -2818,195 +3096,276 @@
       <c r="C12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:5" ht="28.8">
-      <c r="A13" s="60"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="34" t="s">
         <v>112</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="41"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:5" ht="28.8">
-      <c r="A14" s="60"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="34" t="s">
         <v>113</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:5" ht="28.8">
-      <c r="A15" s="60"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="34" t="s">
         <v>114</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:5" ht="28.8">
-      <c r="A16" s="60"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="34" t="s">
         <v>115</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:5" ht="28.8">
-      <c r="A17" s="60"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="34" t="s">
         <v>155</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:5" ht="28.8">
-      <c r="A18" s="60"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="34" t="s">
         <v>169</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:5" ht="28.8">
-      <c r="A19" s="60"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="34" t="s">
         <v>185</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:5" ht="28.8">
-      <c r="A20" s="60"/>
-      <c r="B20" s="49" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="49" t="s">
         <v>184</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="28.8">
-      <c r="A21" s="60"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="34" t="s">
         <v>193</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:5" ht="28.8">
-      <c r="A22" s="60"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="34" t="s">
         <v>194</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="23" spans="1:5" ht="28.8">
-      <c r="A23" s="60"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="34" t="s">
         <v>207</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:5" ht="28.8">
-      <c r="A24" s="60"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="34" t="s">
         <v>208</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:5" ht="28.8">
-      <c r="A25" s="60"/>
-      <c r="B25" s="49" t="s">
+      <c r="A25" s="62"/>
+      <c r="B25" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="49" t="s">
         <v>213</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="28.8">
-      <c r="A26" s="60"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="48" t="s">
         <v>212</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:5" ht="28.8">
-      <c r="A27" s="60"/>
-      <c r="B27" s="49" t="s">
+      <c r="A27" s="62"/>
+      <c r="B27" s="48" t="s">
         <v>212</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:5" ht="28.8">
-      <c r="A28" s="60"/>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="48" t="s">
         <v>212</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D28" s="41"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:5" ht="28.8">
-      <c r="A29" s="60"/>
-      <c r="B29" s="49" t="s">
+      <c r="A29" s="62"/>
+      <c r="B29" s="48" t="s">
         <v>212</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A30" s="61"/>
-      <c r="B30" s="45" t="s">
+      <c r="A30" s="63"/>
+      <c r="B30" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="48"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="47"/>
+    </row>
+    <row r="31" spans="1:5" ht="28.8">
+      <c r="A31" s="61" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" s="40"/>
+    </row>
+    <row r="32" spans="1:5" ht="28.8">
+      <c r="A32" s="62"/>
+      <c r="B32" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32" s="40"/>
+    </row>
+    <row r="33" spans="1:4" ht="28.8">
+      <c r="A33" s="62"/>
+      <c r="B33" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D33" s="40"/>
+    </row>
+    <row r="34" spans="1:4" ht="28.8">
+      <c r="A34" s="62"/>
+      <c r="B34" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D34" s="40"/>
+    </row>
+    <row r="35" spans="1:4" ht="43.2">
+      <c r="A35" s="62"/>
+      <c r="B35" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="40"/>
+    </row>
+    <row r="36" spans="1:4" ht="43.2">
+      <c r="A36" s="62"/>
+      <c r="B36" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D36" s="40"/>
+    </row>
+    <row r="37" spans="1:4" ht="43.2">
+      <c r="A37" s="62"/>
+      <c r="B37" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8">
+      <c r="A38" s="62"/>
+      <c r="B38" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>269</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="A12:A30"/>
+    <mergeCell ref="A31:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3041,17 +3400,17 @@
       <c r="C1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="64"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:29" ht="43.2">
       <c r="A2" s="4" t="s">
@@ -3060,17 +3419,17 @@
       <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="63"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="62"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="4" t="s">
@@ -3974,7 +4333,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4120,8 +4479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5914067F-A3D6-4F1D-8A65-E4F056E7FEB8}">
   <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4139,44 +4498,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="71" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:17" ht="57.6">
-      <c r="A2" s="30" t="s">
+    </row>
+    <row r="3" spans="1:17" ht="57.6">
+      <c r="A3" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="30" t="s">
+    <row r="4" spans="1:17" ht="43.2" customHeight="1">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="43.2" customHeight="1">
-      <c r="B4" s="66" t="s">
+    <row r="5" spans="1:17" ht="43.2">
+      <c r="B5" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="66"/>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="30"/>
+      <c r="C5" s="58"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="57" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4197,7 +4564,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="43.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="57" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -4251,10 +4618,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="58.2" customHeight="1">
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="66"/>
+      <c r="C15" s="70"/>
     </row>
     <row r="16" spans="1:17" ht="14.4" customHeight="1">
       <c r="A16" s="30"/>
@@ -4320,18 +4687,18 @@
       <c r="A24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="64" t="s">
+      <c r="C24" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="65"/>
+      <c r="H24" s="67"/>
       <c r="I24" s="33" t="s">
         <v>155</v>
       </c>
@@ -4343,18 +4710,18 @@
       <c r="A25" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
       <c r="F25" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="63" t="s">
+      <c r="G25" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="63"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="32" t="s">
         <v>170</v>
       </c>
@@ -4422,7 +4789,7 @@
       <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>125</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -4452,7 +4819,7 @@
       <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>126</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -4482,7 +4849,7 @@
       <c r="A34">
         <v>3</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>127</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -4512,7 +4879,7 @@
       <c r="A35">
         <v>4</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="36" t="s">
         <v>128</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -4542,7 +4909,7 @@
       <c r="A36">
         <v>5</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>129</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -4574,7 +4941,7 @@
       <c r="A37">
         <v>6</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="36" t="s">
         <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -4604,7 +4971,7 @@
       <c r="A38">
         <v>7</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>131</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -4636,7 +5003,7 @@
       <c r="A39">
         <v>8</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="36" t="s">
         <v>132</v>
       </c>
       <c r="C39" s="2"/>
@@ -4658,7 +5025,7 @@
       <c r="A40">
         <v>9</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="36" t="s">
         <v>133</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -4682,7 +5049,7 @@
       <c r="A41">
         <v>10</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="36" t="s">
         <v>134</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -4712,7 +5079,7 @@
       <c r="A42">
         <v>11</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="36" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4720,11 +5087,11 @@
       <c r="A44" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C44" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="3" t="s">
         <v>165</v>
       </c>
@@ -4768,35 +5135,35 @@
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
-      <c r="J46" s="44" t="s">
+      <c r="J46" s="43" t="s">
         <v>174</v>
       </c>
       <c r="K46" s="12"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="J47" s="42" t="s">
+      <c r="J47" s="41" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="57.6">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="J48" s="42" t="s">
+      <c r="J48" s="41" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B49" t="s">
@@ -4805,7 +5172,7 @@
       <c r="C49" t="s">
         <v>2</v>
       </c>
-      <c r="J49" s="42" t="s">
+      <c r="J49" s="41" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4813,24 +5180,24 @@
       <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="J50" s="42" t="s">
+      <c r="J50" s="41" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="39"/>
+      <c r="A51" s="38"/>
       <c r="B51" t="s">
         <v>187</v>
       </c>
-      <c r="J51" s="43" t="s">
+      <c r="J51" s="42" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="J52" s="43" t="s">
+      <c r="J52" s="42" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4841,12 +5208,12 @@
       <c r="B53" t="s">
         <v>188</v>
       </c>
-      <c r="J53" s="43" t="s">
+      <c r="J53" s="42" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.2">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -4867,23 +5234,23 @@
       <c r="K56" s="12"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C57" s="38" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="72">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="38" t="s">
+      <c r="C58" s="37" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B59" t="s">
@@ -4899,13 +5266,13 @@
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="39"/>
+      <c r="A61" s="38"/>
       <c r="B61" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="38" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4926,7 +5293,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="43.2">
-      <c r="A66" s="39" t="s">
+      <c r="A66" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -4934,58 +5301,60 @@
       </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="56"/>
-      <c r="B67" s="56"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="56"/>
-      <c r="I67" s="12"/>
+      <c r="A67" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="71"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="I67" s="55"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="39" t="s">
+      <c r="C68" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="D68" s="39" t="s">
+      <c r="D68" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="E68" s="39" t="s">
+      <c r="E68" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="F68" s="39" t="s">
+      <c r="F68" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="G68" s="39" t="s">
+      <c r="G68" s="38" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="57.6">
-      <c r="A69" s="39" t="s">
+      <c r="A69" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="38" t="s">
+      <c r="C69" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D69" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="E69" s="38" t="s">
+      <c r="E69" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="F69" s="38" t="s">
+      <c r="F69" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="G69" s="38" t="s">
+      <c r="G69" s="37" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B71" t="s">
@@ -5001,13 +5370,13 @@
       </c>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="39"/>
+      <c r="A73" s="38"/>
       <c r="B73" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B75" s="2"/>
@@ -5044,7 +5413,7 @@
       <c r="A77">
         <v>2</v>
       </c>
-      <c r="B77" s="40" t="s">
+      <c r="B77" s="39" t="s">
         <v>195</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -5065,7 +5434,7 @@
       <c r="A78">
         <v>3</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="39" t="s">
         <v>196</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -5086,7 +5455,7 @@
       <c r="A79">
         <v>4</v>
       </c>
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="39" t="s">
         <v>197</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -5107,7 +5476,7 @@
       <c r="A80">
         <v>5</v>
       </c>
-      <c r="B80" s="40" t="s">
+      <c r="B80" s="39" t="s">
         <v>198</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -5128,7 +5497,7 @@
       <c r="A81">
         <v>6</v>
       </c>
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="39" t="s">
         <v>199</v>
       </c>
       <c r="C81" s="2"/>
@@ -5145,7 +5514,7 @@
       <c r="A82">
         <v>7</v>
       </c>
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="39" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="2"/>
@@ -5163,62 +5532,64 @@
       <c r="G83" s="2"/>
     </row>
     <row r="84" spans="1:8" ht="57.6">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="40" t="s">
+      <c r="C84" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D84" s="40" t="s">
+      <c r="D84" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="E84" s="40" t="s">
+      <c r="E84" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="F84" s="40" t="s">
+      <c r="F84" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="G84" s="40" t="s">
+      <c r="G84" s="39" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="43.2">
       <c r="B85" s="2"/>
-      <c r="C85" s="40" t="s">
+      <c r="C85" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D85" s="40" t="s">
+      <c r="D85" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="E85" s="40" t="s">
+      <c r="E85" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="F85" s="40" t="s">
+      <c r="F85" s="39" t="s">
         <v>217</v>
       </c>
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="56"/>
-      <c r="B86" s="56"/>
-      <c r="C86" s="56"/>
-      <c r="D86" s="56"/>
-      <c r="E86" s="56"/>
-      <c r="F86" s="56"/>
-      <c r="G86" s="56"/>
-      <c r="H86" s="56"/>
+      <c r="A86" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="71"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="71"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="71"/>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C87" s="39" t="s">
+      <c r="C87" s="38" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="43.2">
-      <c r="A88" s="39" t="s">
+      <c r="A88" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C88" s="7" t="s">
@@ -5226,7 +5597,7 @@
       </c>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B90" t="s">
@@ -5242,13 +5613,13 @@
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="39"/>
+      <c r="A92" s="38"/>
       <c r="B92" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="38" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5261,7 +5632,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="28.8">
-      <c r="A97" s="39" t="s">
+      <c r="A97" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -5279,21 +5650,21 @@
       <c r="H98" s="12"/>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C99" s="39" t="s">
+      <c r="C99" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="D99" s="39" t="s">
+      <c r="D99" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="E99" s="39" t="s">
+      <c r="E99" s="38" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="57.6">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C100" s="7" t="s">
@@ -5313,7 +5684,7 @@
       <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="39" t="s">
+      <c r="A102" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -5334,7 +5705,7 @@
       <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" s="39"/>
+      <c r="A104" s="38"/>
       <c r="B104" s="2" t="s">
         <v>230</v>
       </c>
@@ -5351,7 +5722,7 @@
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:8">
-      <c r="A106" s="39" t="s">
+      <c r="A106" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B106" s="2"/>
@@ -5403,53 +5774,53 @@
       <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:8" ht="57.6">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="2"/>
-      <c r="C111" s="40" t="s">
+      <c r="C111" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="D111" s="40" t="s">
+      <c r="D111" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="E111" s="40" t="s">
+      <c r="E111" s="39" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="12"/>
-      <c r="B112" s="55"/>
-      <c r="C112" s="55"/>
-      <c r="D112" s="55"/>
-      <c r="E112" s="55"/>
+      <c r="B112" s="54"/>
+      <c r="C112" s="54"/>
+      <c r="D112" s="54"/>
+      <c r="E112" s="54"/>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
     </row>
     <row r="113" spans="1:8">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="38" t="s">
         <v>26</v>
       </c>
       <c r="B113" s="2"/>
-      <c r="C113" s="65" t="s">
+      <c r="C113" s="67" t="s">
         <v>241</v>
       </c>
-      <c r="D113" s="65"/>
-      <c r="E113" s="65"/>
+      <c r="D113" s="67"/>
+      <c r="E113" s="67"/>
     </row>
     <row r="114" spans="1:8">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C114" s="67" t="s">
+      <c r="C114" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="D114" s="67"/>
-      <c r="E114" s="67"/>
+      <c r="D114" s="68"/>
+      <c r="E114" s="68"/>
     </row>
     <row r="116" spans="1:8">
-      <c r="A116" s="39" t="s">
+      <c r="A116" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B116" s="2" t="s">
@@ -5466,7 +5837,7 @@
       <c r="C117" s="2"/>
     </row>
     <row r="118" spans="1:8">
-      <c r="A118" s="39"/>
+      <c r="A118" s="38"/>
       <c r="B118" s="2" t="s">
         <v>230</v>
       </c>
@@ -5479,16 +5850,16 @@
       <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:8">
-      <c r="A120" s="39" t="s">
+      <c r="A120" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C120" s="39" t="s">
+      <c r="C120" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D120" s="39" t="s">
+      <c r="D120" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="E120" s="39" t="s">
+      <c r="E120" s="38" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5536,15 +5907,15 @@
       <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:8" ht="27" customHeight="1">
-      <c r="A125" s="39" t="s">
+      <c r="A125" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B125" s="2"/>
-      <c r="C125" s="68" t="s">
+      <c r="C125" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="D125" s="68"/>
-      <c r="E125" s="68"/>
+      <c r="D125" s="69"/>
+      <c r="E125" s="69"/>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" s="12"/>
@@ -5557,23 +5928,23 @@
       <c r="H126" s="12"/>
     </row>
     <row r="127" spans="1:8">
-      <c r="A127" s="39" t="s">
+      <c r="A127" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C127" s="39" t="s">
+      <c r="C127" s="38" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="43.2">
-      <c r="A128" s="39" t="s">
+      <c r="A128" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C128" s="38" t="s">
+      <c r="C128" s="37" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="130" spans="1:8">
-      <c r="A130" s="39" t="s">
+      <c r="A130" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -5590,7 +5961,7 @@
       <c r="C131" s="2"/>
     </row>
     <row r="132" spans="1:8">
-      <c r="A132" s="39"/>
+      <c r="A132" s="38"/>
       <c r="B132" s="2" t="s">
         <v>252</v>
       </c>
@@ -5603,7 +5974,7 @@
       <c r="C133" s="2"/>
     </row>
     <row r="134" spans="1:8">
-      <c r="A134" s="39" t="s">
+      <c r="A134" s="38" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5632,7 +6003,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="57.6">
-      <c r="A139" s="39" t="s">
+      <c r="A139" s="38" t="s">
         <v>8</v>
       </c>
       <c r="C139" s="3" t="s">
@@ -5640,27 +6011,29 @@
       </c>
     </row>
     <row r="140" spans="1:8">
-      <c r="A140" s="56"/>
-      <c r="B140" s="56"/>
-      <c r="C140" s="56"/>
-      <c r="D140" s="56"/>
-      <c r="E140" s="56"/>
-      <c r="F140" s="56"/>
-      <c r="G140" s="56"/>
-      <c r="H140" s="56"/>
+      <c r="A140" s="55"/>
+      <c r="B140" s="55"/>
+      <c r="C140" s="55"/>
+      <c r="D140" s="55"/>
+      <c r="E140" s="55"/>
+      <c r="F140" s="55"/>
+      <c r="G140" s="55"/>
+      <c r="H140" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A67:H67"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C113:E113"/>
     <mergeCell ref="C114:E114"/>
     <mergeCell ref="C125:E125"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="C44:E44"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C113:E113"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C79" r:id="rId1" xr:uid="{A14C5E75-288F-4637-9146-BEA59811E139}"/>
@@ -5671,4 +6044,437 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0661E0-248A-4F53-8703-C8DFF2E40441}">
+  <dimension ref="A1:Q44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="71" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.2">
+      <c r="A3" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="1:17" ht="28.8">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="28.8">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="57.6">
+      <c r="A10" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="28.8">
+      <c r="C11" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="57.6">
+      <c r="A14" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="B16" s="58" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="58"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="57.6">
+      <c r="A21" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="57.6">
+      <c r="A24" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="43.2">
+      <c r="B26" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="57.6">
+      <c r="A31" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="D32" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+    </row>
+    <row r="34" spans="1:17" ht="57.6" customHeight="1">
+      <c r="A34" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="86.4">
+      <c r="A35" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="43.2">
+      <c r="B37" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="C37" s="58"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="E38" s="57" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C40" s="72">
+        <v>6</v>
+      </c>
+      <c r="D40" s="72">
+        <v>0</v>
+      </c>
+      <c r="E40" s="72">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="86.4">
+      <c r="A42" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="C43" s="3"/>
+      <c r="D43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>